<commit_message>
INPUT.NEXTLINE TRIM & COMMENTS
</commit_message>
<xml_diff>
--- a/Movie.xlsx
+++ b/Movie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juancarlosrodriguezflores/Documents/MovieTheatre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA749C8-373C-B14E-85BE-A95CC569C0C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439A865C-8D85-0F45-817C-D3348FAC90BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{00834B12-B30A-1643-9581-5C55C058304C}"/>
   </bookViews>
@@ -639,7 +639,7 @@
   <dimension ref="D5:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>